<commit_message>
Server evauation: Initial version for review
</commit_message>
<xml_diff>
--- a/docs/server technology evaluation - comparison.xlsx
+++ b/docs/server technology evaluation - comparison.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abs\Documents\LEIC\1516v\PS\tertulias\docs\"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="33">
   <si>
     <t>Requirement</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Service maturity (&gt; 5 yrs)</t>
   </si>
   <si>
-    <t>Customer base size</t>
-  </si>
-  <si>
     <t>Relevant mobile Apps using it</t>
   </si>
   <si>
@@ -120,6 +117,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Customer base dimension</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -167,7 +170,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="22">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -210,46 +243,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -269,36 +262,36 @@
   <autoFilter ref="A1:L18"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Requirement" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Weigth" totalsRowDxfId="10"/>
-    <tableColumn id="3" name="AWS" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="9">
-      <totalsRowFormula>IF(AND(C2="Y",SUM(C3:C8)=6),SUMPRODUCT($B9:$B18,C9:C18),"-")</totalsRowFormula>
+    <tableColumn id="2" name="Weigth" totalsRowDxfId="20"/>
+    <tableColumn id="3" name="AWS" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
+      <totalsRowFormula>IF(ISNA(MATCH("N",C2:C8,0)),SUMPRODUCT($B9:$B18,C9:C18),"-")</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="Appcelerator" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="8">
-      <totalsRowFormula>IF(AND(D2="Y",SUM(D3:D8)=6),SUMPRODUCT($B9:$B18,D9:D18),"-")</totalsRowFormula>
+    <tableColumn id="4" name="Appcelerator" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="16">
+      <totalsRowFormula>IF(ISNA(MATCH("N",D2:D8,0)),SUMPRODUCT($B9:$B18,D9:D18),"-")</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="BaasBox" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="7">
-      <totalsRowFormula>IF(AND(E2="Y",SUM(E3:E8)=6),SUMPRODUCT($B9:$B18,E9:E18),"-")</totalsRowFormula>
+    <tableColumn id="5" name="BaasBox" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
+      <totalsRowFormula>IF(ISNA(MATCH("N",E2:E8,0)),SUMPRODUCT($B9:$B18,E9:E18),"-")</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="built.io" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="6">
-      <totalsRowFormula>IF(AND(F2="Y",SUM(F3:F8)=6),SUMPRODUCT($B9:$B18,F9:F18),"-")</totalsRowFormula>
+    <tableColumn id="6" name="built.io" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12">
+      <totalsRowFormula>IF(ISNA(MATCH("N",F2:F8,0)),SUMPRODUCT($B9:$B18,F9:F18),"-")</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="Firebase" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="5">
-      <totalsRowFormula>IF(AND(G2="Y",SUM(G3:G8)=6),SUMPRODUCT($B9:$B18,G9:G18),"-")</totalsRowFormula>
+    <tableColumn id="7" name="Firebase" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+      <totalsRowFormula>IF(ISNA(MATCH("N",G2:G8,0)),SUMPRODUCT($B9:$B18,G9:G18),"-")</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="Azure" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="4">
-      <totalsRowFormula>IF(AND(H2="Y",SUM(H3:H8)=6),SUMPRODUCT($B9:$B18,H9:H18),"-")</totalsRowFormula>
+    <tableColumn id="8" name="Azure" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
+      <totalsRowFormula>IF(ISNA(MATCH("N",H2:H8,0)),SUMPRODUCT($B9:$B18,H9:H18),"-")</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" name="Oracle" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="3">
-      <totalsRowFormula>IF(AND(I2="Y",SUM(I3:I8)=6),SUMPRODUCT($B9:$B18,I9:I18),"-")</totalsRowFormula>
+    <tableColumn id="9" name="Oracle" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
+      <totalsRowFormula>IF(ISNA(MATCH("N",I2:I8,0)),SUMPRODUCT($B9:$B18,I9:I18),"-")</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" name="FeedHenry" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="2">
-      <totalsRowFormula>IF(AND(J2="Y",SUM(J3:J8)=6),SUMPRODUCT($B9:$B18,J9:J18),"-")</totalsRowFormula>
+    <tableColumn id="10" name="FeedHenry" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+      <totalsRowFormula>IF(ISNA(MATCH("N",J2:J8,0)),SUMPRODUCT($B9:$B18,J9:J18),"-")</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" name="StrongLoop" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="1">
-      <totalsRowFormula>IF(AND(K2="Y",SUM(K3:K8)=6),SUMPRODUCT($B9:$B18,K9:K18),"-")</totalsRowFormula>
+    <tableColumn id="11" name="StrongLoop" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
+      <totalsRowFormula>IF(ISNA(MATCH("N",K2:K8,0)),SUMPRODUCT($B9:$B18,K9:K18),"-")</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" name="MongoLab" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="0">
-      <totalsRowFormula>IF(AND(L2="Y",SUM(L3:L8)=6),SUMPRODUCT($B9:$B18,L9:L18),"-")</totalsRowFormula>
+    <tableColumn id="12" name="MongoLab" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
+      <totalsRowFormula>IF(ISNA(MATCH("N",L2:L8,0)),SUMPRODUCT($B9:$B18,L9:L18),"-")</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -570,9 +563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -663,194 +654,230 @@
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1">
-        <v>0</v>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1">
-        <v>0</v>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1">
-        <v>0</v>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1">
-        <v>1</v>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1">
-        <v>1</v>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1">
-        <v>1</v>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -873,16 +900,22 @@
       <c r="H9" s="1">
         <v>1</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
       <c r="L9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1">
         <v>5</v>
@@ -905,16 +938,22 @@
       <c r="H10" s="1">
         <v>1</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
       <c r="L10" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1">
         <v>8</v>
@@ -937,16 +976,22 @@
       <c r="H11" s="1">
         <v>1</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
       <c r="L11" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -969,16 +1014,22 @@
       <c r="H12" s="1">
         <v>1</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
       <c r="L12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1">
         <v>5</v>
@@ -1001,16 +1052,22 @@
       <c r="H13" s="1">
         <v>1</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
       <c r="L13" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1">
         <v>4</v>
@@ -1033,16 +1090,22 @@
       <c r="H14" s="1">
         <v>1</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
       <c r="L14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1">
         <v>8</v>
@@ -1065,16 +1128,22 @@
       <c r="H15" s="1">
         <v>1</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
       <c r="L15" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1">
         <v>3</v>
@@ -1097,16 +1166,22 @@
       <c r="H16" s="1">
         <v>2</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>3</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2</v>
+      </c>
       <c r="L16" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
@@ -1129,16 +1204,22 @@
       <c r="H17" s="1">
         <v>5</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1">
+        <v>2</v>
+      </c>
+      <c r="K17" s="1">
+        <v>3</v>
+      </c>
       <c r="L17" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1">
         <v>5</v>
@@ -1162,13 +1243,13 @@
         <v>5</v>
       </c>
       <c r="I18" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J18" s="1">
         <v>3</v>
       </c>
       <c r="K18" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L18" s="1">
         <v>3</v>
@@ -1176,15 +1257,15 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1">
-        <f>IF(AND(C2="Y",SUM(C3:C8)=6),SUMPRODUCT($B9:$B18,C9:C18),"-")</f>
+        <f>IF(ISNA(MATCH("N",C2:C8,0)),SUMPRODUCT($B9:$B18,C9:C18),"-")</f>
         <v>68</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" ref="D19:L19" si="0">IF(AND(D2="Y",SUM(D3:D8)=6),SUMPRODUCT($B9:$B18,D9:D18),"-")</f>
+        <f t="shared" ref="D19:L19" si="0">IF(ISNA(MATCH("N",D2:D8,0)),SUMPRODUCT($B9:$B18,D9:D18),"-")</f>
         <v>72</v>
       </c>
       <c r="E19" s="1" t="str">
@@ -1207,13 +1288,13 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="J19" s="1" t="str">
+      <c r="J19" s="1">
         <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="K19" s="1" t="str">
+        <v>68</v>
+      </c>
+      <c r="K19" s="1">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>79</v>
       </c>
       <c r="L19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1222,7 +1303,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C19:L19">
-    <cfRule type="top10" dxfId="11" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="21" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>